<commit_message>
Add fonts EA74 to EA87  add new words
Add fonts EA74 to EA87  add new words - convert, wise, think.
Fixed some typos in dictionaries.
</commit_message>
<xml_diff>
--- a/Proper Noun Dictionary (unicode1).xlsx
+++ b/Proper Noun Dictionary (unicode1).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="352">
   <si>
     <t xml:space="preserve">Abiathar</t>
   </si>
@@ -31,6 +31,15 @@
     <t xml:space="preserve">e35f</t>
   </si>
   <si>
+    <t xml:space="preserve">Abijah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea5b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abraham</t>
   </si>
   <si>
@@ -58,6 +67,15 @@
     <t xml:space="preserve">e35d</t>
   </si>
   <si>
+    <t xml:space="preserve">Amminadab</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea51</t>
+  </si>
+  <si>
     <t xml:space="preserve">Andrew</t>
   </si>
   <si>
@@ -76,6 +94,15 @@
     <t xml:space="preserve">e34d</t>
   </si>
   <si>
+    <t xml:space="preserve">Asa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea5c</t>
+  </si>
+  <si>
     <t xml:space="preserve">Barabbas</t>
   </si>
   <si>
@@ -112,6 +139,15 @@
     <t xml:space="preserve">e349</t>
   </si>
   <si>
+    <t xml:space="preserve">Bethlehem</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea45</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bethphage</t>
   </si>
   <si>
@@ -130,6 +166,15 @@
     <t xml:space="preserve">e340</t>
   </si>
   <si>
+    <t xml:space="preserve">Boaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea54</t>
+  </si>
+  <si>
     <t xml:space="preserve">Caesarea</t>
   </si>
   <si>
@@ -139,6 +184,15 @@
     <t xml:space="preserve">e346</t>
   </si>
   <si>
+    <t xml:space="preserve">Caiaphas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea77</t>
+  </si>
+  <si>
     <t xml:space="preserve">Canaan</t>
   </si>
   <si>
@@ -193,6 +247,15 @@
     <t xml:space="preserve">e344</t>
   </si>
   <si>
+    <t xml:space="preserve">Daniel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea78</t>
+  </si>
+  <si>
     <t xml:space="preserve">David</t>
   </si>
   <si>
@@ -211,6 +274,15 @@
     <t xml:space="preserve">e33e</t>
   </si>
   <si>
+    <t xml:space="preserve">Egypt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea44</t>
+  </si>
+  <si>
     <t xml:space="preserve">Elijah</t>
   </si>
   <si>
@@ -220,6 +292,15 @@
     <t xml:space="preserve">e36a</t>
   </si>
   <si>
+    <t xml:space="preserve">Gadarenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">e33f</t>
+  </si>
+  <si>
     <t xml:space="preserve">Galilee</t>
   </si>
   <si>
@@ -241,15 +322,6 @@
     <t xml:space="preserve">Gerasenes</t>
   </si>
   <si>
-    <t xml:space="preserve"></t>
-  </si>
-  <si>
-    <t xml:space="preserve">e33f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gadarenes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gethsemane</t>
   </si>
   <si>
@@ -277,6 +349,15 @@
     <t xml:space="preserve">e34b</t>
   </si>
   <si>
+    <t xml:space="preserve">Gomorrah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea7a</t>
+  </si>
+  <si>
     <t xml:space="preserve">Greece</t>
   </si>
   <si>
@@ -304,6 +385,15 @@
     <t xml:space="preserve">e355</t>
   </si>
   <si>
+    <t xml:space="preserve">Hezron</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea4f</t>
+  </si>
+  <si>
     <t xml:space="preserve">Idumea</t>
   </si>
   <si>
@@ -367,6 +457,24 @@
     <t xml:space="preserve">e376</t>
   </si>
   <si>
+    <t xml:space="preserve">Jehoshaphat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea5d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeremiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea28</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jerusalem</t>
   </si>
   <si>
@@ -376,6 +484,15 @@
     <t xml:space="preserve">e338</t>
   </si>
   <si>
+    <t xml:space="preserve">Jesse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea58</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jesus</t>
   </si>
   <si>
@@ -385,6 +502,15 @@
     <t xml:space="preserve">e037</t>
   </si>
   <si>
+    <t xml:space="preserve">John_the_Baptist</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">e336</t>
+  </si>
+  <si>
     <t xml:space="preserve">John(the_Disciple)</t>
   </si>
   <si>
@@ -394,15 +520,6 @@
     <t xml:space="preserve">e35a</t>
   </si>
   <si>
-    <t xml:space="preserve">John_the_Baptist</t>
-  </si>
-  <si>
-    <t xml:space="preserve"></t>
-  </si>
-  <si>
-    <t xml:space="preserve">e336</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jonah</t>
   </si>
   <si>
@@ -412,6 +529,15 @@
     <t xml:space="preserve">e0c5</t>
   </si>
   <si>
+    <t xml:space="preserve">Joram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea5e</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jordan_River</t>
   </si>
   <si>
@@ -439,6 +565,24 @@
     <t xml:space="preserve">e369</t>
   </si>
   <si>
+    <t xml:space="preserve">Judah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea4b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judas_Iscariot </t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">e365</t>
+  </si>
+  <si>
     <t xml:space="preserve">Judas(not_Iscariot)</t>
   </si>
   <si>
@@ -448,15 +592,6 @@
     <t xml:space="preserve">e368</t>
   </si>
   <si>
-    <t xml:space="preserve">Judas_Iscariot </t>
-  </si>
-  <si>
-    <t xml:space="preserve"></t>
-  </si>
-  <si>
-    <t xml:space="preserve">e365</t>
-  </si>
-  <si>
     <t xml:space="preserve">Judea</t>
   </si>
   <si>
@@ -493,6 +628,15 @@
     <t xml:space="preserve">e371</t>
   </si>
   <si>
+    <t xml:space="preserve">Mary_Magdalene</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">e353</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mary(Mother_of_Jesus)</t>
   </si>
   <si>
@@ -502,15 +646,6 @@
     <t xml:space="preserve">e354</t>
   </si>
   <si>
-    <t xml:space="preserve">Mary_Magdalene</t>
-  </si>
-  <si>
-    <t xml:space="preserve"></t>
-  </si>
-  <si>
-    <t xml:space="preserve">e353</t>
-  </si>
-  <si>
     <t xml:space="preserve">Messiah</t>
   </si>
   <si>
@@ -532,6 +667,30 @@
     <t xml:space="preserve">e351</t>
   </si>
   <si>
+    <t xml:space="preserve">Nahshon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naphatali</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea40</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nazareth</t>
   </si>
   <si>
@@ -550,6 +709,15 @@
     <t xml:space="preserve">e0c6</t>
   </si>
   <si>
+    <t xml:space="preserve">Obed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea56</t>
+  </si>
+  <si>
     <t xml:space="preserve">Paul</t>
   </si>
   <si>
@@ -559,6 +727,15 @@
     <t xml:space="preserve">e377</t>
   </si>
   <si>
+    <t xml:space="preserve">Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea4c</t>
+  </si>
+  <si>
     <t xml:space="preserve">Philip </t>
   </si>
   <si>
@@ -595,6 +772,51 @@
     <t xml:space="preserve">e36f</t>
   </si>
   <si>
+    <t xml:space="preserve">Rachel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rahab</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rehoboam</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea5a</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rufus</t>
   </si>
   <si>
@@ -604,6 +826,24 @@
     <t xml:space="preserve">e36e</t>
   </si>
   <si>
+    <t xml:space="preserve">Ruth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea53</t>
+  </si>
+  <si>
     <t xml:space="preserve">Salome</t>
   </si>
   <si>
@@ -613,6 +853,24 @@
     <t xml:space="preserve">e379</t>
   </si>
   <si>
+    <t xml:space="preserve">Samaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samaritan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea7b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Satan</t>
   </si>
   <si>
@@ -658,6 +916,33 @@
     <t xml:space="preserve">e33c</t>
   </si>
   <si>
+    <t xml:space="preserve">Simon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simon_of_Cyrene</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">e37c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simon_Peter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">e356</t>
+  </si>
+  <si>
     <t xml:space="preserve">Simon_the_Canaanite</t>
   </si>
   <si>
@@ -667,15 +952,6 @@
     <t xml:space="preserve">e364</t>
   </si>
   <si>
-    <t xml:space="preserve">Simon_of_Cyrene</t>
-  </si>
-  <si>
-    <t xml:space="preserve"></t>
-  </si>
-  <si>
-    <t xml:space="preserve">e37c</t>
-  </si>
-  <si>
     <t xml:space="preserve">Simon_the_Leper</t>
   </si>
   <si>
@@ -685,13 +961,13 @@
     <t xml:space="preserve">e0f8</t>
   </si>
   <si>
-    <t xml:space="preserve">Simon_Peter</t>
-  </si>
-  <si>
-    <t xml:space="preserve"></t>
-  </si>
-  <si>
-    <t xml:space="preserve">e356</t>
+    <t xml:space="preserve">Solomon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea32</t>
   </si>
   <si>
     <t xml:space="preserve">Son_of_Man</t>
@@ -712,6 +988,15 @@
     <t xml:space="preserve">e342</t>
   </si>
   <si>
+    <t xml:space="preserve">Tamar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea4e</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thaddaeus</t>
   </si>
   <si>
@@ -748,6 +1033,15 @@
     <t xml:space="preserve">e33b</t>
   </si>
   <si>
+    <t xml:space="preserve">Uriah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea46</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yahweh</t>
   </si>
   <si>
@@ -764,6 +1058,24 @@
   </si>
   <si>
     <t xml:space="preserve">e359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zebulun</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zerah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea4d</t>
   </si>
 </sst>
 </file>
@@ -907,10 +1219,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="57.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -944,7 +1256,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>58227</v>
+        <v>59995</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -957,6 +1269,9 @@
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="1" t="n">
+        <v>58227</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
@@ -969,7 +1284,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>58205</v>
+        <v>59924</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
@@ -983,7 +1298,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>58199</v>
+        <v>58205</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -997,7 +1312,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>58189</v>
+        <v>59985</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -1011,7 +1326,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>58221</v>
+        <v>58199</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>20</v>
@@ -1025,7 +1340,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>58210</v>
+        <v>58189</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>23</v>
@@ -1039,7 +1354,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>58219</v>
+        <v>59996</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>26</v>
@@ -1053,7 +1368,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>58185</v>
+        <v>58221</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>29</v>
@@ -1067,7 +1382,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>58184</v>
+        <v>58210</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>32</v>
@@ -1081,7 +1396,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>58176</v>
+        <v>58219</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>35</v>
@@ -1095,7 +1410,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>58182</v>
+        <v>58185</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>38</v>
@@ -1109,7 +1424,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>58173</v>
+        <v>59973</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>41</v>
@@ -1123,7 +1438,7 @@
         <v>43</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>58170</v>
+        <v>58184</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>44</v>
@@ -1137,7 +1452,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>58224</v>
+        <v>58176</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>47</v>
@@ -1151,7 +1466,7 @@
         <v>49</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>58164</v>
+        <v>59988</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>50</v>
@@ -1165,7 +1480,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>58237</v>
+        <v>58182</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>53</v>
@@ -1179,7 +1494,7 @@
         <v>55</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>58180</v>
+        <v>60023</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>56</v>
@@ -1193,7 +1508,7 @@
         <v>58</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>58206</v>
+        <v>58173</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>59</v>
@@ -1207,7 +1522,7 @@
         <v>61</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>58174</v>
+        <v>58170</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>62</v>
@@ -1221,7 +1536,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>58218</v>
+        <v>58224</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>65</v>
@@ -1235,7 +1550,7 @@
         <v>67</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>58167</v>
+        <v>58164</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>68</v>
@@ -1249,7 +1564,7 @@
         <v>70</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>58177</v>
+        <v>58237</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>71</v>
@@ -1263,7 +1578,7 @@
         <v>73</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>58175</v>
+        <v>58180</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>74</v>
@@ -1274,125 +1589,125 @@
         <v>75</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>58175</v>
+        <v>60024</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>58186</v>
+        <v>58206</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>57398</v>
+        <v>58174</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>58187</v>
+        <v>59972</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>58181</v>
+        <v>58218</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>58208</v>
+        <v>58175</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>58197</v>
+        <v>58167</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>58232</v>
+        <v>58177</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>58228</v>
+        <v>58175</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1403,7 +1718,7 @@
         <v>101</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>58226</v>
+        <v>58186</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>102</v>
@@ -1417,7 +1732,7 @@
         <v>104</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>58229</v>
+        <v>57398</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>105</v>
@@ -1431,7 +1746,7 @@
         <v>107</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>58215</v>
+        <v>58187</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>108</v>
@@ -1445,7 +1760,7 @@
         <v>110</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>58200</v>
+        <v>60026</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>111</v>
@@ -1459,7 +1774,7 @@
         <v>113</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>58230</v>
+        <v>58181</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>114</v>
@@ -1473,7 +1788,7 @@
         <v>116</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>58168</v>
+        <v>58208</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>117</v>
@@ -1487,7 +1802,7 @@
         <v>119</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>57399</v>
+        <v>58197</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>120</v>
@@ -1501,7 +1816,7 @@
         <v>122</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>58202</v>
+        <v>59983</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>123</v>
@@ -1515,7 +1830,7 @@
         <v>125</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>58166</v>
+        <v>58232</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>126</v>
@@ -1528,6 +1843,9 @@
       <c r="B44" s="2" t="s">
         <v>128</v>
       </c>
+      <c r="C44" s="1" t="n">
+        <v>58228</v>
+      </c>
       <c r="D44" s="3" t="s">
         <v>129</v>
       </c>
@@ -1540,7 +1858,7 @@
         <v>131</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>58191</v>
+        <v>58226</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>132</v>
@@ -1553,6 +1871,9 @@
       <c r="B46" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="C46" s="1" t="n">
+        <v>58229</v>
+      </c>
       <c r="D46" s="3" t="s">
         <v>135</v>
       </c>
@@ -1565,7 +1886,7 @@
         <v>137</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>58217</v>
+        <v>58215</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>138</v>
@@ -1579,7 +1900,7 @@
         <v>140</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>58216</v>
+        <v>58200</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>141</v>
@@ -1593,7 +1914,7 @@
         <v>143</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>58213</v>
+        <v>58230</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>144</v>
@@ -1607,7 +1928,7 @@
         <v>146</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>58169</v>
+        <v>59997</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>147</v>
@@ -1621,7 +1942,7 @@
         <v>149</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>58214</v>
+        <v>59944</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>150</v>
@@ -1635,7 +1956,7 @@
         <v>152</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>58204</v>
+        <v>58168</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>153</v>
@@ -1649,7 +1970,7 @@
         <v>155</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>58225</v>
+        <v>59992</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>156</v>
@@ -1663,7 +1984,7 @@
         <v>158</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>58196</v>
+        <v>57399</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>159</v>
@@ -1677,7 +1998,7 @@
         <v>161</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>58195</v>
+        <v>58166</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>162</v>
@@ -1688,217 +2009,223 @@
         <v>163</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>49</v>
+        <v>164</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>58164</v>
+        <v>58202</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>50</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>58203</v>
+        <v>57541</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>58193</v>
+        <v>59998</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>58190</v>
+        <v>58191</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>59925</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>58231</v>
+        <v>58217</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>58209</v>
+        <v>59979</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>58183</v>
+        <v>58213</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>58179</v>
+        <v>58216</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>58223</v>
+        <v>58169</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>58222</v>
+        <v>58214</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>58233</v>
+        <v>58204</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>58165</v>
+        <v>58225</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>57900</v>
+        <v>58195</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>58192</v>
+        <v>58196</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>207</v>
+        <v>67</v>
+      </c>
+      <c r="C71" s="1" t="n">
+        <v>58164</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>208</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,21 +2236,21 @@
         <v>210</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>58172</v>
+        <v>58203</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>213</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>58212</v>
+        <v>58193</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>214</v>
@@ -1934,150 +2261,643 @@
         <v>215</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" s="1" t="n">
+        <v>59986</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="C74" s="1" t="n">
-        <v>58236</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="1" t="n">
+        <v>59976</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="1" t="n">
+        <v>59968</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="C76" s="1" t="n">
-        <v>58198</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="1" t="n">
+        <v>58190</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="C77" s="1" t="n">
-        <v>58194</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="1" t="n">
+        <v>57542</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="C78" s="1" t="n">
-        <v>58178</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="1" t="n">
+        <v>59990</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="C79" s="1" t="n">
-        <v>58235</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="1" t="n">
+        <v>58231</v>
+      </c>
+      <c r="D80" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="C80" s="1" t="n">
-        <v>58211</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="1" t="n">
+        <v>59980</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>237</v>
-      </c>
-      <c r="C81" s="1" t="n">
-        <v>58220</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="1" t="n">
+        <v>58209</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="C82" s="1" t="n">
-        <v>58171</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="1" t="n">
+        <v>58183</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="1" t="n">
+        <v>58179</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C84" s="1" t="n">
+    </row>
+    <row r="85" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>58223</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>59969</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>59989</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C88" s="1" t="n">
+        <v>59984</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>59970</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>59994</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C91" s="1" t="n">
+        <v>58222</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C92" s="1" t="n">
+        <v>59991</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C93" s="1" t="n">
+        <v>59987</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C94" s="1" t="n">
+        <v>58233</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C95" s="1" t="n">
+        <v>60035</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C96" s="1" t="n">
+        <v>60027</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C97" s="1" t="n">
+        <v>58165</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C98" s="1" t="n">
+        <v>57900</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C99" s="1" t="n">
+        <v>58192</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C100" s="1" t="n">
+        <v>57545</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C101" s="1" t="n">
+        <v>58172</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C102" s="1" t="n">
+        <v>59975</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C103" s="1" t="n">
+        <v>58236</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C104" s="1" t="n">
+        <v>58198</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C105" s="1" t="n">
+        <v>58212</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C106" s="1" t="n">
+        <v>57592</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C107" s="1" t="n">
+        <v>59954</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C108" s="1" t="n">
+        <v>58194</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C109" s="1" t="n">
+        <v>58178</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C110" s="1" t="n">
+        <v>59982</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C111" s="1" t="n">
+        <v>58235</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C112" s="1" t="n">
+        <v>58211</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C113" s="1" t="n">
+        <v>58220</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C114" s="1" t="n">
+        <v>58171</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C115" s="1" t="n">
+        <v>59974</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C116" s="1" t="n">
+        <v>57543</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C117" s="1" t="n">
         <v>58201</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>247</v>
+      <c r="D117" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C118" s="1" t="n">
+        <v>59967</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C119" s="1" t="n">
+        <v>59981</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added fonts EA5F to EA73
</commit_message>
<xml_diff>
--- a/Proper Noun Dictionary (unicode1).xlsx
+++ b/Proper Noun Dictionary (unicode1).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="415">
   <si>
     <t xml:space="preserve">Abiathar</t>
   </si>
@@ -40,6 +40,15 @@
     <t xml:space="preserve">ea5b</t>
   </si>
   <si>
+    <t xml:space="preserve">Abiud</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea6a</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abraham</t>
   </si>
   <si>
@@ -49,6 +58,24 @@
     <t xml:space="preserve">e373</t>
   </si>
   <si>
+    <t xml:space="preserve">Achim</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea6e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea61</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alexander</t>
   </si>
   <si>
@@ -76,6 +103,15 @@
     <t xml:space="preserve">ea51</t>
   </si>
   <si>
+    <t xml:space="preserve">Amon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea64</t>
+  </si>
+  <si>
     <t xml:space="preserve">Andrew</t>
   </si>
   <si>
@@ -103,6 +139,24 @@
     <t xml:space="preserve">ea5c</t>
   </si>
   <si>
+    <t xml:space="preserve">Azor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea6c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babylon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea67</t>
+  </si>
+  <si>
     <t xml:space="preserve">Barabbas</t>
   </si>
   <si>
@@ -283,6 +337,24 @@
     <t xml:space="preserve">ea44</t>
   </si>
   <si>
+    <t xml:space="preserve">Eleazar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliakim</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea6b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Elijah</t>
   </si>
   <si>
@@ -292,6 +364,15 @@
     <t xml:space="preserve">e36a</t>
   </si>
   <si>
+    <t xml:space="preserve">Eliud</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea6f</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gadarenes</t>
   </si>
   <si>
@@ -385,6 +466,15 @@
     <t xml:space="preserve">e355</t>
   </si>
   <si>
+    <t xml:space="preserve">Hezekiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea62</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hezron</t>
   </si>
   <si>
@@ -430,6 +520,15 @@
     <t xml:space="preserve">e375</t>
   </si>
   <si>
+    <t xml:space="preserve">(NT)Jacob</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea72</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jairus</t>
   </si>
   <si>
@@ -457,6 +556,15 @@
     <t xml:space="preserve">e358</t>
   </si>
   <si>
+    <t xml:space="preserve">Jechoniah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea66</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jehoshaphat</t>
   </si>
   <si>
@@ -556,6 +664,15 @@
     <t xml:space="preserve">ea15</t>
   </si>
   <si>
+    <t xml:space="preserve">(NT)Joseph</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea73</t>
+  </si>
+  <si>
     <t xml:space="preserve">Joses</t>
   </si>
   <si>
@@ -565,6 +682,24 @@
     <t xml:space="preserve">e369</t>
   </si>
   <si>
+    <t xml:space="preserve">Josiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jothan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea60</t>
+  </si>
+  <si>
     <t xml:space="preserve">Judah</t>
   </si>
   <si>
@@ -619,6 +754,15 @@
     <t xml:space="preserve">e35c</t>
   </si>
   <si>
+    <t xml:space="preserve">Manasseh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea63</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mark</t>
   </si>
   <si>
@@ -646,6 +790,15 @@
     <t xml:space="preserve">e354</t>
   </si>
   <si>
+    <t xml:space="preserve">Matthan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea71</t>
+  </si>
+  <si>
     <t xml:space="preserve">Messiah</t>
   </si>
   <si>
@@ -898,6 +1051,15 @@
     <t xml:space="preserve">e350</t>
   </si>
   <si>
+    <t xml:space="preserve">Shealtiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea68</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sheol</t>
   </si>
   <si>
@@ -1042,6 +1204,15 @@
     <t xml:space="preserve">ea46</t>
   </si>
   <si>
+    <t xml:space="preserve">Uzziah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea5f</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yahweh</t>
   </si>
   <si>
@@ -1051,6 +1222,15 @@
     <t xml:space="preserve">e0c7</t>
   </si>
   <si>
+    <t xml:space="preserve">Zadok</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea6d</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zebedee</t>
   </si>
   <si>
@@ -1076,6 +1256,15 @@
   </si>
   <si>
     <t xml:space="preserve">ea4d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zerubbabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea69</t>
   </si>
 </sst>
 </file>
@@ -1219,10 +1408,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D119" activeCellId="0" sqref="D119"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F73" activeCellId="0" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="57.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1270,7 +1459,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>58227</v>
+        <v>60010</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -1284,7 +1473,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>59924</v>
+        <v>58227</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
@@ -1298,7 +1487,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>58205</v>
+        <v>60014</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -1312,7 +1501,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>59985</v>
+        <v>60001</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -1326,7 +1515,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>58199</v>
+        <v>59924</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>20</v>
@@ -1340,7 +1529,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>58189</v>
+        <v>58205</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>23</v>
@@ -1354,7 +1543,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>59996</v>
+        <v>59985</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>26</v>
@@ -1368,7 +1557,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>58221</v>
+        <v>60004</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>29</v>
@@ -1382,7 +1571,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>58210</v>
+        <v>58199</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>32</v>
@@ -1396,7 +1585,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>58219</v>
+        <v>58189</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>35</v>
@@ -1410,7 +1599,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>58185</v>
+        <v>59996</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>38</v>
@@ -1424,7 +1613,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>59973</v>
+        <v>60012</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>41</v>
@@ -1438,7 +1627,7 @@
         <v>43</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>58184</v>
+        <v>60007</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>44</v>
@@ -1452,7 +1641,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>58176</v>
+        <v>58221</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>47</v>
@@ -1466,7 +1655,7 @@
         <v>49</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>59988</v>
+        <v>58210</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>50</v>
@@ -1480,7 +1669,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>58182</v>
+        <v>58219</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>53</v>
@@ -1494,7 +1683,7 @@
         <v>55</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>60023</v>
+        <v>58185</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>56</v>
@@ -1508,7 +1697,7 @@
         <v>58</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>58173</v>
+        <v>59973</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>59</v>
@@ -1522,7 +1711,7 @@
         <v>61</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>58170</v>
+        <v>58184</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>62</v>
@@ -1536,7 +1725,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>58224</v>
+        <v>58176</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>65</v>
@@ -1550,7 +1739,7 @@
         <v>67</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>58164</v>
+        <v>59988</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>68</v>
@@ -1564,7 +1753,7 @@
         <v>70</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>58237</v>
+        <v>58182</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>71</v>
@@ -1578,7 +1767,7 @@
         <v>73</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>58180</v>
+        <v>60023</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>74</v>
@@ -1592,7 +1781,7 @@
         <v>76</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>60024</v>
+        <v>58173</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>77</v>
@@ -1606,7 +1795,7 @@
         <v>79</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>58206</v>
+        <v>58170</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>80</v>
@@ -1620,7 +1809,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>58174</v>
+        <v>58224</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>83</v>
@@ -1634,7 +1823,7 @@
         <v>85</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>59972</v>
+        <v>58164</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>86</v>
@@ -1648,7 +1837,7 @@
         <v>88</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>58218</v>
+        <v>58237</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>89</v>
@@ -1662,7 +1851,7 @@
         <v>91</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>58175</v>
+        <v>58180</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>92</v>
@@ -1676,7 +1865,7 @@
         <v>94</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>58167</v>
+        <v>60024</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>95</v>
@@ -1690,7 +1879,7 @@
         <v>97</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>58177</v>
+        <v>58206</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>98</v>
@@ -1701,139 +1890,139 @@
         <v>99</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>58175</v>
+        <v>58174</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>58186</v>
+        <v>59972</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>57398</v>
+        <v>60016</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>58187</v>
+        <v>60011</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>60026</v>
+        <v>58218</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>58181</v>
+        <v>60015</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>58208</v>
+        <v>58175</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>58197</v>
+        <v>58167</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>59983</v>
+        <v>58177</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>58232</v>
+        <v>58175</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1844,7 +2033,7 @@
         <v>128</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>58228</v>
+        <v>58186</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>129</v>
@@ -1858,7 +2047,7 @@
         <v>131</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>58226</v>
+        <v>57398</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>132</v>
@@ -1872,7 +2061,7 @@
         <v>134</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>58229</v>
+        <v>58187</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>135</v>
@@ -1886,7 +2075,7 @@
         <v>137</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>58215</v>
+        <v>60026</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>138</v>
@@ -1900,7 +2089,7 @@
         <v>140</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>58200</v>
+        <v>58181</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>141</v>
@@ -1914,7 +2103,7 @@
         <v>143</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>58230</v>
+        <v>58208</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>144</v>
@@ -1928,7 +2117,7 @@
         <v>146</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>59997</v>
+        <v>58197</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>147</v>
@@ -1942,7 +2131,7 @@
         <v>149</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>59944</v>
+        <v>60002</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>150</v>
@@ -1956,7 +2145,7 @@
         <v>152</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>58168</v>
+        <v>59983</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>153</v>
@@ -1970,7 +2159,7 @@
         <v>155</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>59992</v>
+        <v>58232</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>156</v>
@@ -1984,7 +2173,7 @@
         <v>158</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>57399</v>
+        <v>58228</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>159</v>
@@ -1998,7 +2187,7 @@
         <v>161</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>58166</v>
+        <v>58226</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>162</v>
@@ -2012,7 +2201,7 @@
         <v>164</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>58202</v>
+        <v>58229</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>165</v>
@@ -2026,7 +2215,7 @@
         <v>167</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>57541</v>
+        <v>60018</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>168</v>
@@ -2040,7 +2229,7 @@
         <v>170</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>59998</v>
+        <v>58215</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>171</v>
@@ -2054,7 +2243,7 @@
         <v>173</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>58191</v>
+        <v>58200</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>174</v>
@@ -2068,7 +2257,7 @@
         <v>176</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>59925</v>
+        <v>58230</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>177</v>
@@ -2082,7 +2271,7 @@
         <v>179</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>58217</v>
+        <v>60006</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>180</v>
@@ -2096,7 +2285,7 @@
         <v>182</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>59979</v>
+        <v>59997</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>183</v>
@@ -2110,7 +2299,7 @@
         <v>185</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>58213</v>
+        <v>59944</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>186</v>
@@ -2124,7 +2313,7 @@
         <v>188</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>58216</v>
+        <v>58168</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>189</v>
@@ -2138,7 +2327,7 @@
         <v>191</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>58169</v>
+        <v>59992</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>192</v>
@@ -2152,7 +2341,7 @@
         <v>194</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>58214</v>
+        <v>57399</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>195</v>
@@ -2166,7 +2355,7 @@
         <v>197</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>58204</v>
+        <v>58166</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>198</v>
@@ -2180,7 +2369,7 @@
         <v>200</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>58225</v>
+        <v>58202</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>201</v>
@@ -2194,7 +2383,7 @@
         <v>203</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>58195</v>
+        <v>57541</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>204</v>
@@ -2208,7 +2397,7 @@
         <v>206</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>58196</v>
+        <v>59998</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>207</v>
@@ -2219,290 +2408,290 @@
         <v>208</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>67</v>
+        <v>209</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>58164</v>
+        <v>58191</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>68</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>58203</v>
+        <v>59925</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>58193</v>
+        <v>60019</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>16</v>
+        <v>218</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>59986</v>
+        <v>58217</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>59976</v>
+        <v>60005</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>59968</v>
+        <v>60000</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>58190</v>
+        <v>59979</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>57542</v>
+        <v>58213</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>59990</v>
+        <v>58216</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>58231</v>
+        <v>58169</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>59980</v>
+        <v>58214</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>58209</v>
+        <v>58204</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>58183</v>
+        <v>60003</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>58179</v>
+        <v>58225</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>58223</v>
+        <v>58195</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>59969</v>
+        <v>58196</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>59989</v>
+        <v>60017</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>257</v>
+        <v>85</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>59984</v>
+        <v>58164</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>258</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>59970</v>
+        <v>58203</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>59994</v>
+        <v>58193</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>266</v>
+        <v>25</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>58222</v>
+        <v>59986</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>267</v>
@@ -2516,7 +2705,7 @@
         <v>269</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>59991</v>
+        <v>59976</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>270</v>
@@ -2530,7 +2719,7 @@
         <v>272</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>59987</v>
+        <v>59968</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>273</v>
@@ -2544,7 +2733,7 @@
         <v>275</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>58233</v>
+        <v>58190</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>276</v>
@@ -2558,7 +2747,7 @@
         <v>278</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>60035</v>
+        <v>57542</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>279</v>
@@ -2572,7 +2761,7 @@
         <v>281</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>60027</v>
+        <v>59990</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>282</v>
@@ -2586,7 +2775,7 @@
         <v>284</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>58165</v>
+        <v>58231</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>285</v>
@@ -2600,7 +2789,7 @@
         <v>287</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>57900</v>
+        <v>59980</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>288</v>
@@ -2614,7 +2803,7 @@
         <v>290</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>58192</v>
+        <v>58209</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>291</v>
@@ -2628,7 +2817,7 @@
         <v>293</v>
       </c>
       <c r="C100" s="1" t="n">
-        <v>57545</v>
+        <v>58183</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>294</v>
@@ -2642,7 +2831,7 @@
         <v>296</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>58172</v>
+        <v>58179</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>297</v>
@@ -2656,7 +2845,7 @@
         <v>299</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>59975</v>
+        <v>58223</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>300</v>
@@ -2670,7 +2859,7 @@
         <v>302</v>
       </c>
       <c r="C103" s="1" t="n">
-        <v>58236</v>
+        <v>59969</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>303</v>
@@ -2684,21 +2873,21 @@
         <v>305</v>
       </c>
       <c r="C104" s="1" t="n">
-        <v>58198</v>
+        <v>59989</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="1" t="s">
         <v>307</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>308</v>
       </c>
       <c r="C105" s="1" t="n">
-        <v>58212</v>
+        <v>59984</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>309</v>
@@ -2712,7 +2901,7 @@
         <v>311</v>
       </c>
       <c r="C106" s="1" t="n">
-        <v>57592</v>
+        <v>59970</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>312</v>
@@ -2726,7 +2915,7 @@
         <v>314</v>
       </c>
       <c r="C107" s="1" t="n">
-        <v>59954</v>
+        <v>59994</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>315</v>
@@ -2740,7 +2929,7 @@
         <v>317</v>
       </c>
       <c r="C108" s="1" t="n">
-        <v>58194</v>
+        <v>58222</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>318</v>
@@ -2754,7 +2943,7 @@
         <v>320</v>
       </c>
       <c r="C109" s="1" t="n">
-        <v>58178</v>
+        <v>59991</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>321</v>
@@ -2768,7 +2957,7 @@
         <v>323</v>
       </c>
       <c r="C110" s="1" t="n">
-        <v>59982</v>
+        <v>59987</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>324</v>
@@ -2782,7 +2971,7 @@
         <v>326</v>
       </c>
       <c r="C111" s="1" t="n">
-        <v>58235</v>
+        <v>58233</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>327</v>
@@ -2796,7 +2985,7 @@
         <v>329</v>
       </c>
       <c r="C112" s="1" t="n">
-        <v>58211</v>
+        <v>60035</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>330</v>
@@ -2810,7 +2999,7 @@
         <v>332</v>
       </c>
       <c r="C113" s="1" t="n">
-        <v>58220</v>
+        <v>60027</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>333</v>
@@ -2824,7 +3013,7 @@
         <v>335</v>
       </c>
       <c r="C114" s="1" t="n">
-        <v>58171</v>
+        <v>58165</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>336</v>
@@ -2838,7 +3027,7 @@
         <v>338</v>
       </c>
       <c r="C115" s="1" t="n">
-        <v>59974</v>
+        <v>57900</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>339</v>
@@ -2852,7 +3041,7 @@
         <v>341</v>
       </c>
       <c r="C116" s="1" t="n">
-        <v>57543</v>
+        <v>58192</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>342</v>
@@ -2866,7 +3055,7 @@
         <v>344</v>
       </c>
       <c r="C117" s="1" t="n">
-        <v>58201</v>
+        <v>60008</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>345</v>
@@ -2880,7 +3069,7 @@
         <v>347</v>
       </c>
       <c r="C118" s="1" t="n">
-        <v>59967</v>
+        <v>57545</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>348</v>
@@ -2894,10 +3083,304 @@
         <v>350</v>
       </c>
       <c r="C119" s="1" t="n">
-        <v>59981</v>
+        <v>58172</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>351</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C120" s="1" t="n">
+        <v>59975</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C121" s="1" t="n">
+        <v>58236</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C122" s="1" t="n">
+        <v>58198</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C123" s="1" t="n">
+        <v>58212</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C124" s="1" t="n">
+        <v>57592</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C125" s="1" t="n">
+        <v>59954</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C126" s="1" t="n">
+        <v>58194</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C127" s="1" t="n">
+        <v>58178</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C128" s="1" t="n">
+        <v>59982</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C129" s="1" t="n">
+        <v>58235</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C130" s="1" t="n">
+        <v>58211</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C131" s="1" t="n">
+        <v>58220</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C132" s="1" t="n">
+        <v>58171</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C133" s="1" t="n">
+        <v>59974</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C134" s="1" t="n">
+        <v>59999</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C135" s="1" t="n">
+        <v>57543</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C136" s="1" t="n">
+        <v>60013</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C137" s="1" t="n">
+        <v>58201</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C138" s="1" t="n">
+        <v>59967</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C139" s="1" t="n">
+        <v>59981</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C140" s="1" t="n">
+        <v>60009</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added EA88 to EA9D Definitions
Fixed missing definitions
</commit_message>
<xml_diff>
--- a/Proper Noun Dictionary (unicode1).xlsx
+++ b/Proper Noun Dictionary (unicode1).xlsx
@@ -20,7 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="448">
+  <si>
+    <t xml:space="preserve">Abel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea96</t>
+  </si>
   <si>
     <t xml:space="preserve">Abiathar</t>
   </si>
@@ -166,6 +175,15 @@
     <t xml:space="preserve">e36d</t>
   </si>
   <si>
+    <t xml:space="preserve">Barachiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea97</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bartholomew</t>
   </si>
   <si>
@@ -274,6 +292,15 @@
     <t xml:space="preserve">e370</t>
   </si>
   <si>
+    <t xml:space="preserve">Chorazin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea8f</t>
+  </si>
+  <si>
     <t xml:space="preserve">Christ</t>
   </si>
   <si>
@@ -457,6 +484,15 @@
     <t xml:space="preserve">e360</t>
   </si>
   <si>
+    <t xml:space="preserve">Herodians</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea05</t>
+  </si>
+  <si>
     <t xml:space="preserve">Herodias</t>
   </si>
   <si>
@@ -511,6 +547,15 @@
     <t xml:space="preserve">e372</t>
   </si>
   <si>
+    <t xml:space="preserve">Israel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea04</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jacob</t>
   </si>
   <si>
@@ -583,6 +628,15 @@
     <t xml:space="preserve">ea28</t>
   </si>
   <si>
+    <t xml:space="preserve">Jericho</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea99</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jerusalem</t>
   </si>
   <si>
@@ -637,6 +691,15 @@
     <t xml:space="preserve">e0c5</t>
   </si>
   <si>
+    <t xml:space="preserve">Jonah(Simon’s_father)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea29</t>
+  </si>
+  <si>
     <t xml:space="preserve">Joram</t>
   </si>
   <si>
@@ -754,6 +817,15 @@
     <t xml:space="preserve">e35c</t>
   </si>
   <si>
+    <t xml:space="preserve">Magadan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea30</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manasseh</t>
   </si>
   <si>
@@ -1096,6 +1168,15 @@
     <t xml:space="preserve">e37c</t>
   </si>
   <si>
+    <t xml:space="preserve">Simon(Jesus’_Brother)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea92</t>
+  </si>
+  <si>
     <t xml:space="preserve">Simon_Peter</t>
   </si>
   <si>
@@ -1123,6 +1204,15 @@
     <t xml:space="preserve">e0f8</t>
   </si>
   <si>
+    <t xml:space="preserve">Sodom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea8e</t>
+  </si>
+  <si>
     <t xml:space="preserve">Solomon</t>
   </si>
   <si>
@@ -1247,6 +1337,15 @@
   </si>
   <si>
     <t xml:space="preserve">ea3f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zechariah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea98</t>
   </si>
   <si>
     <t xml:space="preserve">Zerah</t>
@@ -1403,15 +1502,628 @@
 </styleSheet>
 </file>
 
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{796F942D-6616-4E33-AD9F-919B2391CE6D}">
+  <header guid="{796F942D-6616-4E33-AD9F-919B2391CE6D}" dateTime="2018-08-22T16:48:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="55" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rrc rId="1" ua="true" sId="1" eol="0" ref="149:149" action="insertRow"/>
+  <rrc rId="2" ua="true" sId="1" eol="0" ref="134:134" action="insertRow"/>
+  <rrc rId="3" ua="true" sId="1" eol="0" ref="130:130" action="insertRow"/>
+  <rrc rId="4" ua="true" sId="1" eol="0" ref="90:90" action="insertRow"/>
+  <rrc rId="5" ua="true" sId="1" eol="0" ref="76:76" action="insertRow"/>
+  <rrc rId="6" ua="true" sId="1" eol="0" ref="69:69" action="insertRow"/>
+  <rrc rId="7" ua="true" sId="1" eol="0" ref="60:60" action="insertRow"/>
+  <rrc rId="8" ua="true" sId="1" eol="0" ref="53:53" action="insertRow"/>
+  <rrc rId="9" ua="true" sId="1" eol="0" ref="31:31" action="insertRow"/>
+  <rrc rId="10" ua="true" sId="1" eol="0" ref="18:18" action="insertRow"/>
+  <rrc rId="11" ua="true" sId="1" eol="0" ref="1:1" action="insertRow"/>
+  <rcc rId="12" ua="true" sId="1">
+    <nc r="A1" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Abel</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="13" ua="true" sId="1">
+    <nc r="B1" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="14" ua="true" sId="1">
+    <nc r="C1" t="n">
+      <v>60054</v>
+    </nc>
+  </rcc>
+  <rcc rId="15" ua="true" sId="1">
+    <nc r="D1" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea96</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="16" ua="true" sId="1">
+    <nc r="A18" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Barachiah</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="17" ua="true" sId="1">
+    <nc r="B18" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="18" ua="true" sId="1">
+    <nc r="C18" t="n">
+      <v>60055</v>
+    </nc>
+  </rcc>
+  <rcc rId="19" ua="true" sId="1">
+    <nc r="D18" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea97</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="20" ua="true" sId="1">
+    <nc r="A31" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Chorazin</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="21" ua="true" sId="1">
+    <nc r="B31" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="22" ua="true" sId="1">
+    <nc r="C31" t="n">
+      <v>60047</v>
+    </nc>
+  </rcc>
+  <rcc rId="23" ua="true" sId="1">
+    <nc r="D31" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea8f</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="24" ua="true" sId="1">
+    <nc r="A53" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Herodians</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="25" ua="true" sId="1">
+    <nc r="B53" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="26" ua="true" sId="1">
+    <nc r="C53" t="n">
+      <v>59909</v>
+    </nc>
+  </rcc>
+  <rcc rId="27" ua="true" sId="1">
+    <nc r="D53" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea05</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="28" ua="true" sId="1">
+    <nc r="A60" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Israel</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="29" ua="true" sId="1">
+    <nc r="B60" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="30" ua="true" sId="1">
+    <nc r="C60" t="n">
+      <v>59908</v>
+    </nc>
+  </rcc>
+  <rcc rId="31" ua="true" sId="1">
+    <nc r="D60" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea04</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="32" ua="true" sId="1">
+    <nc r="A69" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Jericho</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="33" ua="true" sId="1">
+    <nc r="B69" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="34" ua="true" sId="1">
+    <nc r="C69" t="n">
+      <v>60057</v>
+    </nc>
+  </rcc>
+  <rcc rId="35" ua="true" sId="1">
+    <nc r="D69" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea99</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="36" ua="true" sId="1">
+    <nc r="A76" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Jonah(Simon’s_father)</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="37" ua="true" sId="1">
+    <nc r="B76" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="38" ua="true" sId="1">
+    <nc r="C76" t="n">
+      <v>59945</v>
+    </nc>
+  </rcc>
+  <rcc rId="39" ua="true" sId="1">
+    <nc r="D76" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea29</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="40" ua="true" sId="1">
+    <nc r="A90" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Magadan</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="41" ua="true" sId="1">
+    <nc r="B90" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="42" ua="true" sId="1">
+    <nc r="C90" t="n">
+      <v>59952</v>
+    </nc>
+  </rcc>
+  <rcc rId="43" ua="true" sId="1">
+    <nc r="D90" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea30</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="44" ua="true" sId="1">
+    <nc r="A130" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Simon(Jesus’_Brother)</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="45" ua="true" sId="1">
+    <nc r="B130" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="46" ua="true" sId="1">
+    <nc r="C130" t="n">
+      <v>60050</v>
+    </nc>
+  </rcc>
+  <rcc rId="47" ua="true" sId="1">
+    <nc r="D130" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea92</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="48" ua="true" sId="1">
+    <nc r="A134" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Sodom</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="49" ua="true" sId="1">
+    <nc r="B134" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="50" ua="true" sId="1">
+    <nc r="C134" t="n">
+      <v>60046</v>
+    </nc>
+  </rcc>
+  <rcc rId="51" ua="true" sId="1">
+    <nc r="D134" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea8e</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="52" ua="true" sId="1">
+    <nc r="A149" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Zechariah</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="53" ua="true" sId="1">
+    <nc r="B149" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="54" ua="true" sId="1">
+    <nc r="C149" t="n">
+      <v>60056</v>
+    </nc>
+  </rcc>
+  <rcc rId="55" ua="true" sId="1">
+    <nc r="D149" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea98</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D140"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F73" activeCellId="0" sqref="F73"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="57.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1431,7 +2143,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>58207</v>
+        <v>60054</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -1445,7 +2157,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>59995</v>
+        <v>58207</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -1459,7 +2171,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>60010</v>
+        <v>59995</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -1473,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>58227</v>
+        <v>60010</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
@@ -1487,7 +2199,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>60014</v>
+        <v>58227</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -1501,7 +2213,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>60001</v>
+        <v>60014</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -1515,7 +2227,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>59924</v>
+        <v>60001</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>20</v>
@@ -1529,7 +2241,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>58205</v>
+        <v>59924</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>23</v>
@@ -1543,7 +2255,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>59985</v>
+        <v>58205</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>26</v>
@@ -1557,7 +2269,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>60004</v>
+        <v>59985</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>29</v>
@@ -1571,7 +2283,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>58199</v>
+        <v>60004</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>32</v>
@@ -1585,7 +2297,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>58189</v>
+        <v>58199</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>35</v>
@@ -1599,7 +2311,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>59996</v>
+        <v>58189</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>38</v>
@@ -1613,7 +2325,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>60012</v>
+        <v>59996</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>41</v>
@@ -1627,7 +2339,7 @@
         <v>43</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>60007</v>
+        <v>60012</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>44</v>
@@ -1641,7 +2353,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>58221</v>
+        <v>60007</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>47</v>
@@ -1655,7 +2367,7 @@
         <v>49</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>58210</v>
+        <v>58221</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>50</v>
@@ -1669,7 +2381,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>58219</v>
+        <v>60055</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>53</v>
@@ -1683,7 +2395,7 @@
         <v>55</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>58185</v>
+        <v>58210</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>56</v>
@@ -1697,7 +2409,7 @@
         <v>58</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>59973</v>
+        <v>58219</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>59</v>
@@ -1711,7 +2423,7 @@
         <v>61</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>58184</v>
+        <v>58185</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>62</v>
@@ -1725,7 +2437,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>58176</v>
+        <v>59973</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>65</v>
@@ -1739,7 +2451,7 @@
         <v>67</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>59988</v>
+        <v>58184</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>68</v>
@@ -1753,7 +2465,7 @@
         <v>70</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>58182</v>
+        <v>58176</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>71</v>
@@ -1767,7 +2479,7 @@
         <v>73</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>60023</v>
+        <v>59988</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>74</v>
@@ -1781,7 +2493,7 @@
         <v>76</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>58173</v>
+        <v>58182</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>77</v>
@@ -1795,7 +2507,7 @@
         <v>79</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>58170</v>
+        <v>60023</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>80</v>
@@ -1809,7 +2521,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>58224</v>
+        <v>58173</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>83</v>
@@ -1823,7 +2535,7 @@
         <v>85</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>58164</v>
+        <v>58170</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>86</v>
@@ -1837,7 +2549,7 @@
         <v>88</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>58237</v>
+        <v>58224</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>89</v>
@@ -1851,7 +2563,7 @@
         <v>91</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>58180</v>
+        <v>60047</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>92</v>
@@ -1865,7 +2577,7 @@
         <v>94</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>60024</v>
+        <v>58164</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>95</v>
@@ -1879,7 +2591,7 @@
         <v>97</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>58206</v>
+        <v>58237</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>98</v>
@@ -1893,7 +2605,7 @@
         <v>100</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>58174</v>
+        <v>58180</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>101</v>
@@ -1907,7 +2619,7 @@
         <v>103</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>59972</v>
+        <v>60024</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>104</v>
@@ -1921,7 +2633,7 @@
         <v>106</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>60016</v>
+        <v>58206</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>107</v>
@@ -1935,7 +2647,7 @@
         <v>109</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>60011</v>
+        <v>58174</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>110</v>
@@ -1949,7 +2661,7 @@
         <v>112</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>58218</v>
+        <v>59972</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>113</v>
@@ -1963,7 +2675,7 @@
         <v>115</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>60015</v>
+        <v>60016</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>116</v>
@@ -1977,7 +2689,7 @@
         <v>118</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>58175</v>
+        <v>60011</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>119</v>
@@ -1991,7 +2703,7 @@
         <v>121</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>58167</v>
+        <v>58218</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>122</v>
@@ -2005,7 +2717,7 @@
         <v>124</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>58177</v>
+        <v>60015</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>125</v>
@@ -2016,55 +2728,55 @@
         <v>126</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>58175</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>58186</v>
+        <v>58167</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>57398</v>
+        <v>58177</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>58187</v>
+        <v>58175</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2075,7 +2787,7 @@
         <v>137</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>60026</v>
+        <v>58186</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>138</v>
@@ -2089,7 +2801,7 @@
         <v>140</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>58181</v>
+        <v>57398</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>141</v>
@@ -2103,7 +2815,7 @@
         <v>143</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>58208</v>
+        <v>58187</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>144</v>
@@ -2117,7 +2829,7 @@
         <v>146</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>58197</v>
+        <v>60026</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>147</v>
@@ -2131,7 +2843,7 @@
         <v>149</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>60002</v>
+        <v>58181</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>150</v>
@@ -2145,7 +2857,7 @@
         <v>152</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>59983</v>
+        <v>58208</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>153</v>
@@ -2159,7 +2871,7 @@
         <v>155</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>58232</v>
+        <v>59909</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>156</v>
@@ -2173,7 +2885,7 @@
         <v>158</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>58228</v>
+        <v>58197</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>159</v>
@@ -2187,7 +2899,7 @@
         <v>161</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>58226</v>
+        <v>60002</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>162</v>
@@ -2201,7 +2913,7 @@
         <v>164</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>58229</v>
+        <v>59983</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>165</v>
@@ -2215,7 +2927,7 @@
         <v>167</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>60018</v>
+        <v>58232</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>168</v>
@@ -2229,7 +2941,7 @@
         <v>170</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>58215</v>
+        <v>58228</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>171</v>
@@ -2243,7 +2955,7 @@
         <v>173</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>58200</v>
+        <v>58226</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>174</v>
@@ -2257,7 +2969,7 @@
         <v>176</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>58230</v>
+        <v>59908</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>177</v>
@@ -2271,7 +2983,7 @@
         <v>179</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>60006</v>
+        <v>58229</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>180</v>
@@ -2285,7 +2997,7 @@
         <v>182</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>59997</v>
+        <v>60018</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>183</v>
@@ -2299,7 +3011,7 @@
         <v>185</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>59944</v>
+        <v>58215</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>186</v>
@@ -2313,7 +3025,7 @@
         <v>188</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>58168</v>
+        <v>58200</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>189</v>
@@ -2327,7 +3039,7 @@
         <v>191</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>59992</v>
+        <v>58230</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>192</v>
@@ -2341,7 +3053,7 @@
         <v>194</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>57399</v>
+        <v>60006</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>195</v>
@@ -2355,7 +3067,7 @@
         <v>197</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>58166</v>
+        <v>59997</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>198</v>
@@ -2369,7 +3081,7 @@
         <v>200</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>58202</v>
+        <v>59944</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>201</v>
@@ -2383,7 +3095,7 @@
         <v>203</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>57541</v>
+        <v>60057</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>204</v>
@@ -2397,7 +3109,7 @@
         <v>206</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>59998</v>
+        <v>58168</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>207</v>
@@ -2411,7 +3123,7 @@
         <v>209</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>58191</v>
+        <v>59992</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>210</v>
@@ -2425,7 +3137,7 @@
         <v>212</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>59925</v>
+        <v>57399</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>213</v>
@@ -2439,7 +3151,7 @@
         <v>215</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>60019</v>
+        <v>58166</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>216</v>
@@ -2453,7 +3165,7 @@
         <v>218</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>58217</v>
+        <v>58202</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>219</v>
@@ -2467,7 +3179,7 @@
         <v>221</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>60005</v>
+        <v>57541</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>222</v>
@@ -2481,7 +3193,7 @@
         <v>224</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>60000</v>
+        <v>59945</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>225</v>
@@ -2495,7 +3207,7 @@
         <v>227</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>59979</v>
+        <v>59998</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>228</v>
@@ -2509,7 +3221,7 @@
         <v>230</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>58213</v>
+        <v>58191</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>231</v>
@@ -2523,7 +3235,7 @@
         <v>233</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>58216</v>
+        <v>59925</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>234</v>
@@ -2537,7 +3249,7 @@
         <v>236</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>58169</v>
+        <v>60019</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>237</v>
@@ -2551,7 +3263,7 @@
         <v>239</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>58214</v>
+        <v>58217</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>240</v>
@@ -2565,7 +3277,7 @@
         <v>242</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>58204</v>
+        <v>60005</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>243</v>
@@ -2579,7 +3291,7 @@
         <v>245</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>60003</v>
+        <v>60000</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>246</v>
@@ -2593,7 +3305,7 @@
         <v>248</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>58225</v>
+        <v>59979</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>249</v>
@@ -2607,7 +3319,7 @@
         <v>251</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>58195</v>
+        <v>58213</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>252</v>
@@ -2621,7 +3333,7 @@
         <v>254</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>58196</v>
+        <v>58216</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>255</v>
@@ -2635,7 +3347,7 @@
         <v>257</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>60017</v>
+        <v>58169</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>258</v>
@@ -2646,164 +3358,164 @@
         <v>259</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>85</v>
+        <v>260</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>58164</v>
+        <v>58214</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>86</v>
+        <v>261</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>58203</v>
+        <v>58204</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>58193</v>
+        <v>59952</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>25</v>
+        <v>269</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>59986</v>
+        <v>60003</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>59976</v>
+        <v>58225</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>59968</v>
+        <v>58195</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>58190</v>
+        <v>58196</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>57542</v>
+        <v>60017</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>281</v>
+        <v>94</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>59990</v>
+        <v>58164</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>282</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>58231</v>
+        <v>58203</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>59980</v>
+        <v>58193</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>290</v>
+        <v>28</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>58209</v>
+        <v>59986</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>291</v>
@@ -2817,7 +3529,7 @@
         <v>293</v>
       </c>
       <c r="C100" s="1" t="n">
-        <v>58183</v>
+        <v>59976</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>294</v>
@@ -2831,7 +3543,7 @@
         <v>296</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>58179</v>
+        <v>59968</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>297</v>
@@ -2845,7 +3557,7 @@
         <v>299</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>58223</v>
+        <v>58190</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>300</v>
@@ -2859,7 +3571,7 @@
         <v>302</v>
       </c>
       <c r="C103" s="1" t="n">
-        <v>59969</v>
+        <v>57542</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>303</v>
@@ -2873,7 +3585,7 @@
         <v>305</v>
       </c>
       <c r="C104" s="1" t="n">
-        <v>59989</v>
+        <v>59990</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>306</v>
@@ -2887,7 +3599,7 @@
         <v>308</v>
       </c>
       <c r="C105" s="1" t="n">
-        <v>59984</v>
+        <v>58231</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>309</v>
@@ -2901,7 +3613,7 @@
         <v>311</v>
       </c>
       <c r="C106" s="1" t="n">
-        <v>59970</v>
+        <v>59980</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>312</v>
@@ -2915,7 +3627,7 @@
         <v>314</v>
       </c>
       <c r="C107" s="1" t="n">
-        <v>59994</v>
+        <v>58209</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>315</v>
@@ -2929,7 +3641,7 @@
         <v>317</v>
       </c>
       <c r="C108" s="1" t="n">
-        <v>58222</v>
+        <v>58183</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>318</v>
@@ -2943,7 +3655,7 @@
         <v>320</v>
       </c>
       <c r="C109" s="1" t="n">
-        <v>59991</v>
+        <v>58179</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>321</v>
@@ -2957,7 +3669,7 @@
         <v>323</v>
       </c>
       <c r="C110" s="1" t="n">
-        <v>59987</v>
+        <v>58223</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>324</v>
@@ -2971,7 +3683,7 @@
         <v>326</v>
       </c>
       <c r="C111" s="1" t="n">
-        <v>58233</v>
+        <v>59969</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>327</v>
@@ -2985,7 +3697,7 @@
         <v>329</v>
       </c>
       <c r="C112" s="1" t="n">
-        <v>60035</v>
+        <v>59989</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>330</v>
@@ -2999,7 +3711,7 @@
         <v>332</v>
       </c>
       <c r="C113" s="1" t="n">
-        <v>60027</v>
+        <v>59984</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>333</v>
@@ -3013,7 +3725,7 @@
         <v>335</v>
       </c>
       <c r="C114" s="1" t="n">
-        <v>58165</v>
+        <v>59970</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>336</v>
@@ -3027,7 +3739,7 @@
         <v>338</v>
       </c>
       <c r="C115" s="1" t="n">
-        <v>57900</v>
+        <v>59994</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>339</v>
@@ -3041,7 +3753,7 @@
         <v>341</v>
       </c>
       <c r="C116" s="1" t="n">
-        <v>58192</v>
+        <v>58222</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>342</v>
@@ -3055,7 +3767,7 @@
         <v>344</v>
       </c>
       <c r="C117" s="1" t="n">
-        <v>60008</v>
+        <v>59991</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>345</v>
@@ -3069,7 +3781,7 @@
         <v>347</v>
       </c>
       <c r="C118" s="1" t="n">
-        <v>57545</v>
+        <v>59987</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>348</v>
@@ -3083,7 +3795,7 @@
         <v>350</v>
       </c>
       <c r="C119" s="1" t="n">
-        <v>58172</v>
+        <v>58233</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>351</v>
@@ -3097,7 +3809,7 @@
         <v>353</v>
       </c>
       <c r="C120" s="1" t="n">
-        <v>59975</v>
+        <v>60035</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>354</v>
@@ -3111,7 +3823,7 @@
         <v>356</v>
       </c>
       <c r="C121" s="1" t="n">
-        <v>58236</v>
+        <v>60027</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>357</v>
@@ -3125,21 +3837,21 @@
         <v>359</v>
       </c>
       <c r="C122" s="1" t="n">
-        <v>58198</v>
+        <v>58165</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="4" t="s">
+      <c r="A123" s="1" t="s">
         <v>361</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>362</v>
       </c>
       <c r="C123" s="1" t="n">
-        <v>58212</v>
+        <v>57900</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>363</v>
@@ -3153,7 +3865,7 @@
         <v>365</v>
       </c>
       <c r="C124" s="1" t="n">
-        <v>57592</v>
+        <v>58192</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>366</v>
@@ -3167,7 +3879,7 @@
         <v>368</v>
       </c>
       <c r="C125" s="1" t="n">
-        <v>59954</v>
+        <v>60008</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>369</v>
@@ -3181,7 +3893,7 @@
         <v>371</v>
       </c>
       <c r="C126" s="1" t="n">
-        <v>58194</v>
+        <v>57545</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>372</v>
@@ -3195,7 +3907,7 @@
         <v>374</v>
       </c>
       <c r="C127" s="1" t="n">
-        <v>58178</v>
+        <v>58172</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>375</v>
@@ -3209,7 +3921,7 @@
         <v>377</v>
       </c>
       <c r="C128" s="1" t="n">
-        <v>59982</v>
+        <v>59975</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>378</v>
@@ -3223,7 +3935,7 @@
         <v>380</v>
       </c>
       <c r="C129" s="1" t="n">
-        <v>58235</v>
+        <v>58236</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>381</v>
@@ -3237,7 +3949,7 @@
         <v>383</v>
       </c>
       <c r="C130" s="1" t="n">
-        <v>58211</v>
+        <v>60050</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>384</v>
@@ -3251,21 +3963,21 @@
         <v>386</v>
       </c>
       <c r="C131" s="1" t="n">
-        <v>58220</v>
+        <v>58198</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="s">
+      <c r="A132" s="4" t="s">
         <v>388</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>389</v>
       </c>
       <c r="C132" s="1" t="n">
-        <v>58171</v>
+        <v>58212</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>390</v>
@@ -3279,7 +3991,7 @@
         <v>392</v>
       </c>
       <c r="C133" s="1" t="n">
-        <v>59974</v>
+        <v>57592</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>393</v>
@@ -3293,7 +4005,7 @@
         <v>395</v>
       </c>
       <c r="C134" s="1" t="n">
-        <v>59999</v>
+        <v>60046</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>396</v>
@@ -3307,7 +4019,7 @@
         <v>398</v>
       </c>
       <c r="C135" s="1" t="n">
-        <v>57543</v>
+        <v>59954</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>399</v>
@@ -3321,7 +4033,7 @@
         <v>401</v>
       </c>
       <c r="C136" s="1" t="n">
-        <v>60013</v>
+        <v>58194</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>402</v>
@@ -3335,7 +4047,7 @@
         <v>404</v>
       </c>
       <c r="C137" s="1" t="n">
-        <v>58201</v>
+        <v>58178</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>405</v>
@@ -3349,7 +4061,7 @@
         <v>407</v>
       </c>
       <c r="C138" s="1" t="n">
-        <v>59967</v>
+        <v>59982</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>408</v>
@@ -3363,7 +4075,7 @@
         <v>410</v>
       </c>
       <c r="C139" s="1" t="n">
-        <v>59981</v>
+        <v>58235</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>411</v>
@@ -3377,10 +4089,164 @@
         <v>413</v>
       </c>
       <c r="C140" s="1" t="n">
-        <v>60009</v>
+        <v>58211</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>414</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C141" s="1" t="n">
+        <v>58220</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C142" s="1" t="n">
+        <v>58171</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C143" s="1" t="n">
+        <v>59974</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C144" s="1" t="n">
+        <v>59999</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C145" s="1" t="n">
+        <v>57543</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C146" s="1" t="n">
+        <v>60013</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C147" s="1" t="n">
+        <v>58201</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C148" s="1" t="n">
+        <v>59967</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C149" s="1" t="n">
+        <v>60056</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="C150" s="1" t="n">
+        <v>59981</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C151" s="1" t="n">
+        <v>60009</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed spelling for EA92 to Simon(Jesus's_brother)
</commit_message>
<xml_diff>
--- a/Proper Noun Dictionary (unicode1).xlsx
+++ b/Proper Noun Dictionary (unicode1).xlsx
@@ -1168,7 +1168,7 @@
     <t xml:space="preserve">e37c</t>
   </si>
   <si>
-    <t xml:space="preserve">Simon(Jesus’_Brother)</t>
+    <t xml:space="preserve">Simon(Jesus’s_brother)</t>
   </si>
   <si>
     <t xml:space="preserve"></t>
@@ -1373,7 +1373,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1424,6 +1424,12 @@
       <color rgb="FF000000"/>
       <name val="Arial Black"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1503,8 +1509,13 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{796F942D-6616-4E33-AD9F-919B2391CE6D}">
-  <header guid="{796F942D-6616-4E33-AD9F-919B2391CE6D}" dateTime="2018-08-22T16:48:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="55" maxSheetId="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{8877E920-E75A-43AA-8A08-0CA0245B3F7A}">
+  <header guid="{6F53D671-456F-4984-AAC5-C8CEA7725BA4}" dateTime="2018-08-22T16:48:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="55" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8877E920-E75A-43AA-8A08-0CA0245B3F7A}" dateTime="2018-08-23T09:28:00.000000000Z" userName=" " r:id="rId2" minRId="56" maxRId="56" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -1514,26 +1525,25 @@
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rrc rId="1" ua="true" sId="1" eol="0" ref="149:149" action="insertRow"/>
-  <rrc rId="2" ua="true" sId="1" eol="0" ref="134:134" action="insertRow"/>
-  <rrc rId="3" ua="true" sId="1" eol="0" ref="130:130" action="insertRow"/>
-  <rrc rId="4" ua="true" sId="1" eol="0" ref="90:90" action="insertRow"/>
-  <rrc rId="5" ua="true" sId="1" eol="0" ref="76:76" action="insertRow"/>
-  <rrc rId="6" ua="true" sId="1" eol="0" ref="69:69" action="insertRow"/>
-  <rrc rId="7" ua="true" sId="1" eol="0" ref="60:60" action="insertRow"/>
-  <rrc rId="8" ua="true" sId="1" eol="0" ref="53:53" action="insertRow"/>
-  <rrc rId="9" ua="true" sId="1" eol="0" ref="31:31" action="insertRow"/>
-  <rrc rId="10" ua="true" sId="1" eol="0" ref="18:18" action="insertRow"/>
-  <rrc rId="11" ua="true" sId="1" eol="0" ref="1:1" action="insertRow"/>
-  <rcc rId="12" ua="true" sId="1">
+  <rrc rId="1" ua="false" sId="1" eol="0" ref="159:159" action="insertRow"/>
+  <rrc rId="2" ua="false" sId="1" eol="0" ref="143:143" action="insertRow"/>
+  <rrc rId="3" ua="false" sId="1" eol="0" ref="138:138" action="insertRow"/>
+  <rrc rId="4" ua="false" sId="1" eol="0" ref="97:97" action="insertRow"/>
+  <rrc rId="5" ua="false" sId="1" eol="0" ref="82:82" action="insertRow"/>
+  <rrc rId="6" ua="false" sId="1" eol="0" ref="74:74" action="insertRow"/>
+  <rrc rId="7" ua="false" sId="1" eol="0" ref="64:64" action="insertRow"/>
+  <rrc rId="8" ua="false" sId="1" eol="0" ref="56:56" action="insertRow"/>
+  <rrc rId="9" ua="false" sId="1" eol="0" ref="33:33" action="insertRow"/>
+  <rrc rId="10" ua="false" sId="1" eol="0" ref="19:19" action="insertRow"/>
+  <rrc rId="11" ua="false" sId="1" eol="0" ref="1:1" action="insertRow"/>
+  <rcc rId="12" ua="false" sId="1">
     <nc r="A1" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Abel</t>
@@ -1541,15 +1551,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="13" ua="true" sId="1">
+  <rcc rId="13" ua="false" sId="1">
     <nc r="B1" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve"></t>
@@ -1557,20 +1566,19 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="14" ua="true" sId="1">
+  <rcc rId="14" ua="false" sId="1">
     <nc r="C1" t="n">
       <v>60054</v>
     </nc>
   </rcc>
-  <rcc rId="15" ua="true" sId="1">
+  <rcc rId="15" ua="false" sId="1">
     <nc r="D1" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">ea96</t>
@@ -1578,15 +1586,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="16" ua="true" sId="1">
+  <rcc rId="16" ua="false" sId="1">
     <nc r="A18" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Barachiah</t>
@@ -1594,15 +1601,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="17" ua="true" sId="1">
+  <rcc rId="17" ua="false" sId="1">
     <nc r="B18" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve"></t>
@@ -1610,20 +1616,19 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="18" ua="true" sId="1">
+  <rcc rId="18" ua="false" sId="1">
     <nc r="C18" t="n">
       <v>60055</v>
     </nc>
   </rcc>
-  <rcc rId="19" ua="true" sId="1">
+  <rcc rId="19" ua="false" sId="1">
     <nc r="D18" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">ea97</t>
@@ -1631,15 +1636,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="20" ua="true" sId="1">
+  <rcc rId="20" ua="false" sId="1">
     <nc r="A31" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Chorazin</t>
@@ -1647,15 +1651,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="21" ua="true" sId="1">
+  <rcc rId="21" ua="false" sId="1">
     <nc r="B31" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve"></t>
@@ -1663,20 +1666,19 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="22" ua="true" sId="1">
+  <rcc rId="22" ua="false" sId="1">
     <nc r="C31" t="n">
       <v>60047</v>
     </nc>
   </rcc>
-  <rcc rId="23" ua="true" sId="1">
+  <rcc rId="23" ua="false" sId="1">
     <nc r="D31" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">ea8f</t>
@@ -1684,15 +1686,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="24" ua="true" sId="1">
+  <rcc rId="24" ua="false" sId="1">
     <nc r="A53" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Herodians</t>
@@ -1700,15 +1701,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="25" ua="true" sId="1">
+  <rcc rId="25" ua="false" sId="1">
     <nc r="B53" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve"></t>
@@ -1716,20 +1716,19 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="26" ua="true" sId="1">
+  <rcc rId="26" ua="false" sId="1">
     <nc r="C53" t="n">
       <v>59909</v>
     </nc>
   </rcc>
-  <rcc rId="27" ua="true" sId="1">
+  <rcc rId="27" ua="false" sId="1">
     <nc r="D53" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">ea05</t>
@@ -1737,15 +1736,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="28" ua="true" sId="1">
+  <rcc rId="28" ua="false" sId="1">
     <nc r="A60" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Israel</t>
@@ -1753,15 +1751,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="29" ua="true" sId="1">
+  <rcc rId="29" ua="false" sId="1">
     <nc r="B60" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve"></t>
@@ -1769,20 +1766,19 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="30" ua="true" sId="1">
+  <rcc rId="30" ua="false" sId="1">
     <nc r="C60" t="n">
       <v>59908</v>
     </nc>
   </rcc>
-  <rcc rId="31" ua="true" sId="1">
+  <rcc rId="31" ua="false" sId="1">
     <nc r="D60" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">ea04</t>
@@ -1790,15 +1786,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="32" ua="true" sId="1">
+  <rcc rId="32" ua="false" sId="1">
     <nc r="A69" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Jericho</t>
@@ -1806,15 +1801,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="33" ua="true" sId="1">
+  <rcc rId="33" ua="false" sId="1">
     <nc r="B69" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve"></t>
@@ -1822,20 +1816,19 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="34" ua="true" sId="1">
+  <rcc rId="34" ua="false" sId="1">
     <nc r="C69" t="n">
       <v>60057</v>
     </nc>
   </rcc>
-  <rcc rId="35" ua="true" sId="1">
+  <rcc rId="35" ua="false" sId="1">
     <nc r="D69" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">ea99</t>
@@ -1843,15 +1836,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="36" ua="true" sId="1">
+  <rcc rId="36" ua="false" sId="1">
     <nc r="A76" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Jonah(Simon’s_father)</t>
@@ -1859,15 +1851,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="37" ua="true" sId="1">
+  <rcc rId="37" ua="false" sId="1">
     <nc r="B76" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve"></t>
@@ -1875,20 +1866,19 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="38" ua="true" sId="1">
+  <rcc rId="38" ua="false" sId="1">
     <nc r="C76" t="n">
       <v>59945</v>
     </nc>
   </rcc>
-  <rcc rId="39" ua="true" sId="1">
+  <rcc rId="39" ua="false" sId="1">
     <nc r="D76" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">ea29</t>
@@ -1896,15 +1886,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="40" ua="true" sId="1">
+  <rcc rId="40" ua="false" sId="1">
     <nc r="A90" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Magadan</t>
@@ -1912,15 +1901,14 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="41" ua="true" sId="1">
+  <rcc rId="41" ua="false" sId="1">
     <nc r="B90" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve"></t>
@@ -1928,20 +1916,19 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="42" ua="true" sId="1">
+  <rcc rId="42" ua="false" sId="1">
     <nc r="C90" t="n">
       <v>59952</v>
     </nc>
   </rcc>
-  <rcc rId="43" ua="true" sId="1">
+  <rcc rId="43" ua="false" sId="1">
     <nc r="D90" t="inlineStr">
       <is>
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">ea30</t>
@@ -1949,8 +1936,163 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="44" ua="true" sId="1">
+  <rcc rId="44" ua="false" sId="1">
     <nc r="A130" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Simon(Jesus’_Brother)</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="45" ua="false" sId="1">
+    <nc r="B130" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="46" ua="false" sId="1">
+    <nc r="C130" t="n">
+      <v>60050</v>
+    </nc>
+  </rcc>
+  <rcc rId="47" ua="false" sId="1">
+    <nc r="D130" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea92</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="48" ua="false" sId="1">
+    <nc r="A134" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Sodom</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="49" ua="false" sId="1">
+    <nc r="B134" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="50" ua="false" sId="1">
+    <nc r="C134" t="n">
+      <v>60046</v>
+    </nc>
+  </rcc>
+  <rcc rId="51" ua="false" sId="1">
+    <nc r="D134" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea8e</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="52" ua="false" sId="1">
+    <nc r="A149" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Zechariah</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="53" ua="false" sId="1">
+    <nc r="B149" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"></t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="54" ua="false" sId="1">
+    <nc r="C149" t="n">
+      <v>60056</v>
+    </nc>
+  </rcc>
+  <rcc rId="55" ua="false" sId="1">
+    <nc r="D149" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea98</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="56" ua="false" sId="1">
+    <oc r="A130" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -1963,10 +2105,8 @@
           <t xml:space="preserve">Simon(Jesus’_Brother)</t>
         </r>
       </is>
-    </nc>
-  </rcc>
-  <rcc rId="45" ua="true" sId="1">
-    <nc r="B130" t="inlineStr">
+    </oc>
+    <nc r="A130" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -1976,134 +2116,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve"></t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="46" ua="true" sId="1">
-    <nc r="C130" t="n">
-      <v>60050</v>
-    </nc>
-  </rcc>
-  <rcc rId="47" ua="true" sId="1">
-    <nc r="D130" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">ea92</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="48" ua="true" sId="1">
-    <nc r="A134" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Sodom</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="49" ua="true" sId="1">
-    <nc r="B134" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve"></t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="50" ua="true" sId="1">
-    <nc r="C134" t="n">
-      <v>60046</v>
-    </nc>
-  </rcc>
-  <rcc rId="51" ua="true" sId="1">
-    <nc r="D134" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">ea8e</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="52" ua="true" sId="1">
-    <nc r="A149" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Zechariah</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="53" ua="true" sId="1">
-    <nc r="B149" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve"></t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="54" ua="true" sId="1">
-    <nc r="C149" t="n">
-      <v>60056</v>
-    </nc>
-  </rcc>
-  <rcc rId="55" ua="true" sId="1">
-    <nc r="D149" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">ea98</t>
+          <t xml:space="preserve">Simon(Jesus’s_brother)</t>
         </r>
       </is>
     </nc>
@@ -2122,8 +2135,8 @@
   </sheetPr>
   <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B132" activeCellId="0" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="57.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added some suggested procedure files
</commit_message>
<xml_diff>
--- a/Proper Noun Dictionary (unicode1).xlsx
+++ b/Proper Noun Dictionary (unicode1).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="451">
   <si>
     <t xml:space="preserve">Abel</t>
   </si>
@@ -932,6 +932,15 @@
   </si>
   <si>
     <t xml:space="preserve">e0c6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">ea43</t>
   </si>
   <si>
     <t xml:space="preserve">Obed</t>
@@ -1509,13 +1518,23 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{8877E920-E75A-43AA-8A08-0CA0245B3F7A}">
-  <header guid="{6F53D671-456F-4984-AAC5-C8CEA7725BA4}" dateTime="2018-08-22T16:48:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="55" maxSheetId="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{9BA6374C-279C-4354-8F60-35DD3333BD39}">
+  <header guid="{D4AA83B9-6A8F-4EF7-9077-C5C7714D311E}" dateTime="2018-08-22T16:48:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="55" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{8877E920-E75A-43AA-8A08-0CA0245B3F7A}" dateTime="2018-08-23T09:28:00.000000000Z" userName=" " r:id="rId2" minRId="56" maxRId="56" maxSheetId="2">
+  <header guid="{E8A03B13-6FD0-4AB8-8D12-18313A00E48C}" dateTime="2018-08-23T09:28:00.000000000Z" userName=" " r:id="rId2" minRId="56" maxRId="56" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E9690B14-03D5-4742-9C0B-9FB635AB68A4}" dateTime="2018-08-23T16:56:00.000000000Z" userName=" " r:id="rId3" minRId="57" maxRId="59" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{9BA6374C-279C-4354-8F60-35DD3333BD39}" dateTime="2018-08-23T16:57:00.000000000Z" userName=" " r:id="rId4" minRId="60" maxRId="61" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -1525,16 +1544,16 @@
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rrc rId="1" ua="false" sId="1" eol="0" ref="159:159" action="insertRow"/>
-  <rrc rId="2" ua="false" sId="1" eol="0" ref="143:143" action="insertRow"/>
-  <rrc rId="3" ua="false" sId="1" eol="0" ref="138:138" action="insertRow"/>
-  <rrc rId="4" ua="false" sId="1" eol="0" ref="97:97" action="insertRow"/>
-  <rrc rId="5" ua="false" sId="1" eol="0" ref="82:82" action="insertRow"/>
-  <rrc rId="6" ua="false" sId="1" eol="0" ref="74:74" action="insertRow"/>
-  <rrc rId="7" ua="false" sId="1" eol="0" ref="64:64" action="insertRow"/>
-  <rrc rId="8" ua="false" sId="1" eol="0" ref="56:56" action="insertRow"/>
-  <rrc rId="9" ua="false" sId="1" eol="0" ref="33:33" action="insertRow"/>
-  <rrc rId="10" ua="false" sId="1" eol="0" ref="19:19" action="insertRow"/>
+  <rrc rId="1" ua="false" sId="1" eol="0" ref="170:170" action="insertRow"/>
+  <rrc rId="2" ua="false" sId="1" eol="0" ref="153:153" action="insertRow"/>
+  <rrc rId="3" ua="false" sId="1" eol="0" ref="147:147" action="insertRow"/>
+  <rrc rId="4" ua="false" sId="1" eol="0" ref="105:105" action="insertRow"/>
+  <rrc rId="5" ua="false" sId="1" eol="0" ref="88:88" action="insertRow"/>
+  <rrc rId="6" ua="false" sId="1" eol="0" ref="79:79" action="insertRow"/>
+  <rrc rId="7" ua="false" sId="1" eol="0" ref="68:68" action="insertRow"/>
+  <rrc rId="8" ua="false" sId="1" eol="0" ref="59:59" action="insertRow"/>
+  <rrc rId="9" ua="false" sId="1" eol="0" ref="35:35" action="insertRow"/>
+  <rrc rId="10" ua="false" sId="1" eol="0" ref="20:20" action="insertRow"/>
   <rrc rId="11" ua="false" sId="1" eol="0" ref="1:1" action="insertRow"/>
   <rcc rId="12" ua="false" sId="1">
     <nc r="A1" t="inlineStr">
@@ -1937,7 +1956,7 @@
     </nc>
   </rcc>
   <rcc rId="44" ua="false" sId="1">
-    <nc r="A130" t="inlineStr">
+    <nc r="A131" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -1952,7 +1971,7 @@
     </nc>
   </rcc>
   <rcc rId="45" ua="false" sId="1">
-    <nc r="B130" t="inlineStr">
+    <nc r="B131" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -1967,12 +1986,12 @@
     </nc>
   </rcc>
   <rcc rId="46" ua="false" sId="1">
-    <nc r="C130" t="n">
+    <nc r="C131" t="n">
       <v>60050</v>
     </nc>
   </rcc>
   <rcc rId="47" ua="false" sId="1">
-    <nc r="D130" t="inlineStr">
+    <nc r="D131" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -1987,7 +2006,7 @@
     </nc>
   </rcc>
   <rcc rId="48" ua="false" sId="1">
-    <nc r="A134" t="inlineStr">
+    <nc r="A135" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2002,7 +2021,7 @@
     </nc>
   </rcc>
   <rcc rId="49" ua="false" sId="1">
-    <nc r="B134" t="inlineStr">
+    <nc r="B135" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2017,12 +2036,12 @@
     </nc>
   </rcc>
   <rcc rId="50" ua="false" sId="1">
-    <nc r="C134" t="n">
+    <nc r="C135" t="n">
       <v>60046</v>
     </nc>
   </rcc>
   <rcc rId="51" ua="false" sId="1">
-    <nc r="D134" t="inlineStr">
+    <nc r="D135" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2037,7 +2056,7 @@
     </nc>
   </rcc>
   <rcc rId="52" ua="false" sId="1">
-    <nc r="A149" t="inlineStr">
+    <nc r="A150" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2052,7 +2071,7 @@
     </nc>
   </rcc>
   <rcc rId="53" ua="false" sId="1">
-    <nc r="B149" t="inlineStr">
+    <nc r="B150" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2067,12 +2086,12 @@
     </nc>
   </rcc>
   <rcc rId="54" ua="false" sId="1">
-    <nc r="C149" t="n">
+    <nc r="C150" t="n">
       <v>60056</v>
     </nc>
   </rcc>
   <rcc rId="55" ua="false" sId="1">
-    <nc r="D149" t="inlineStr">
+    <nc r="D150" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2092,7 +2111,41 @@
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rcc rId="56" ua="false" sId="1">
-    <oc r="A130" t="inlineStr">
+    <oc r="A131" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Simon(Jesus’_Brother)</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="A131" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Simon(Jesus’s_brother)</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rrc rId="57" ua="false" sId="1" eol="0" ref="104:104" action="insertRow"/>
+  <rcc rId="58" ua="false" sId="1">
+    <nc r="A104" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2102,11 +2155,13 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Simon(Jesus’_Brother)</t>
+          <t xml:space="preserve">Noah</t>
         </r>
       </is>
-    </oc>
-    <nc r="A130" t="inlineStr">
+    </nc>
+  </rcc>
+  <rcc rId="59" ua="false" sId="1">
+    <nc r="B104" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2116,9 +2171,35 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Simon(Jesus’s_brother)</t>
+          <t xml:space="preserve"></t>
         </r>
       </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="60" ua="false" sId="1">
+    <nc r="D104" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ea43</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="61" ua="false" sId="1">
+    <nc r="C104" t="n">
+      <v>59971</v>
     </nc>
   </rcc>
 </revisions>
@@ -2133,10 +2214,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D151"/>
+  <dimension ref="A1:D152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B132" activeCellId="0" sqref="B132"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B105" activeCellId="0" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="57.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3598,7 +3679,7 @@
         <v>305</v>
       </c>
       <c r="C104" s="1" t="n">
-        <v>59990</v>
+        <v>59971</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>306</v>
@@ -3612,7 +3693,7 @@
         <v>308</v>
       </c>
       <c r="C105" s="1" t="n">
-        <v>58231</v>
+        <v>59990</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>309</v>
@@ -3626,7 +3707,7 @@
         <v>311</v>
       </c>
       <c r="C106" s="1" t="n">
-        <v>59980</v>
+        <v>58231</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>312</v>
@@ -3640,7 +3721,7 @@
         <v>314</v>
       </c>
       <c r="C107" s="1" t="n">
-        <v>58209</v>
+        <v>59980</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>315</v>
@@ -3654,7 +3735,7 @@
         <v>317</v>
       </c>
       <c r="C108" s="1" t="n">
-        <v>58183</v>
+        <v>58209</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>318</v>
@@ -3668,7 +3749,7 @@
         <v>320</v>
       </c>
       <c r="C109" s="1" t="n">
-        <v>58179</v>
+        <v>58183</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>321</v>
@@ -3682,7 +3763,7 @@
         <v>323</v>
       </c>
       <c r="C110" s="1" t="n">
-        <v>58223</v>
+        <v>58179</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>324</v>
@@ -3696,7 +3777,7 @@
         <v>326</v>
       </c>
       <c r="C111" s="1" t="n">
-        <v>59969</v>
+        <v>58223</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>327</v>
@@ -3710,7 +3791,7 @@
         <v>329</v>
       </c>
       <c r="C112" s="1" t="n">
-        <v>59989</v>
+        <v>59969</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>330</v>
@@ -3724,7 +3805,7 @@
         <v>332</v>
       </c>
       <c r="C113" s="1" t="n">
-        <v>59984</v>
+        <v>59989</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>333</v>
@@ -3738,7 +3819,7 @@
         <v>335</v>
       </c>
       <c r="C114" s="1" t="n">
-        <v>59970</v>
+        <v>59984</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>336</v>
@@ -3752,7 +3833,7 @@
         <v>338</v>
       </c>
       <c r="C115" s="1" t="n">
-        <v>59994</v>
+        <v>59970</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>339</v>
@@ -3766,7 +3847,7 @@
         <v>341</v>
       </c>
       <c r="C116" s="1" t="n">
-        <v>58222</v>
+        <v>59994</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>342</v>
@@ -3780,7 +3861,7 @@
         <v>344</v>
       </c>
       <c r="C117" s="1" t="n">
-        <v>59991</v>
+        <v>58222</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>345</v>
@@ -3794,7 +3875,7 @@
         <v>347</v>
       </c>
       <c r="C118" s="1" t="n">
-        <v>59987</v>
+        <v>59991</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>348</v>
@@ -3808,7 +3889,7 @@
         <v>350</v>
       </c>
       <c r="C119" s="1" t="n">
-        <v>58233</v>
+        <v>59987</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>351</v>
@@ -3822,7 +3903,7 @@
         <v>353</v>
       </c>
       <c r="C120" s="1" t="n">
-        <v>60035</v>
+        <v>58233</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>354</v>
@@ -3836,7 +3917,7 @@
         <v>356</v>
       </c>
       <c r="C121" s="1" t="n">
-        <v>60027</v>
+        <v>60035</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>357</v>
@@ -3850,7 +3931,7 @@
         <v>359</v>
       </c>
       <c r="C122" s="1" t="n">
-        <v>58165</v>
+        <v>60027</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>360</v>
@@ -3864,7 +3945,7 @@
         <v>362</v>
       </c>
       <c r="C123" s="1" t="n">
-        <v>57900</v>
+        <v>58165</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>363</v>
@@ -3878,7 +3959,7 @@
         <v>365</v>
       </c>
       <c r="C124" s="1" t="n">
-        <v>58192</v>
+        <v>57900</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>366</v>
@@ -3892,7 +3973,7 @@
         <v>368</v>
       </c>
       <c r="C125" s="1" t="n">
-        <v>60008</v>
+        <v>58192</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>369</v>
@@ -3906,7 +3987,7 @@
         <v>371</v>
       </c>
       <c r="C126" s="1" t="n">
-        <v>57545</v>
+        <v>60008</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>372</v>
@@ -3920,7 +4001,7 @@
         <v>374</v>
       </c>
       <c r="C127" s="1" t="n">
-        <v>58172</v>
+        <v>57545</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>375</v>
@@ -3934,7 +4015,7 @@
         <v>377</v>
       </c>
       <c r="C128" s="1" t="n">
-        <v>59975</v>
+        <v>58172</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>378</v>
@@ -3948,7 +4029,7 @@
         <v>380</v>
       </c>
       <c r="C129" s="1" t="n">
-        <v>58236</v>
+        <v>59975</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>381</v>
@@ -3962,7 +4043,7 @@
         <v>383</v>
       </c>
       <c r="C130" s="1" t="n">
-        <v>60050</v>
+        <v>58236</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>384</v>
@@ -3976,35 +4057,35 @@
         <v>386</v>
       </c>
       <c r="C131" s="1" t="n">
-        <v>58198</v>
+        <v>60050</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="4" t="s">
+      <c r="A132" s="1" t="s">
         <v>388</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>389</v>
       </c>
       <c r="C132" s="1" t="n">
-        <v>58212</v>
+        <v>58198</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="s">
+      <c r="A133" s="4" t="s">
         <v>391</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>392</v>
       </c>
       <c r="C133" s="1" t="n">
-        <v>57592</v>
+        <v>58212</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>393</v>
@@ -4018,7 +4099,7 @@
         <v>395</v>
       </c>
       <c r="C134" s="1" t="n">
-        <v>60046</v>
+        <v>57592</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>396</v>
@@ -4032,7 +4113,7 @@
         <v>398</v>
       </c>
       <c r="C135" s="1" t="n">
-        <v>59954</v>
+        <v>60046</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>399</v>
@@ -4046,7 +4127,7 @@
         <v>401</v>
       </c>
       <c r="C136" s="1" t="n">
-        <v>58194</v>
+        <v>59954</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>402</v>
@@ -4060,7 +4141,7 @@
         <v>404</v>
       </c>
       <c r="C137" s="1" t="n">
-        <v>58178</v>
+        <v>58194</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>405</v>
@@ -4074,7 +4155,7 @@
         <v>407</v>
       </c>
       <c r="C138" s="1" t="n">
-        <v>59982</v>
+        <v>58178</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>408</v>
@@ -4088,7 +4169,7 @@
         <v>410</v>
       </c>
       <c r="C139" s="1" t="n">
-        <v>58235</v>
+        <v>59982</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>411</v>
@@ -4102,7 +4183,7 @@
         <v>413</v>
       </c>
       <c r="C140" s="1" t="n">
-        <v>58211</v>
+        <v>58235</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>414</v>
@@ -4116,7 +4197,7 @@
         <v>416</v>
       </c>
       <c r="C141" s="1" t="n">
-        <v>58220</v>
+        <v>58211</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>417</v>
@@ -4130,7 +4211,7 @@
         <v>419</v>
       </c>
       <c r="C142" s="1" t="n">
-        <v>58171</v>
+        <v>58220</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>420</v>
@@ -4144,7 +4225,7 @@
         <v>422</v>
       </c>
       <c r="C143" s="1" t="n">
-        <v>59974</v>
+        <v>58171</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>423</v>
@@ -4158,7 +4239,7 @@
         <v>425</v>
       </c>
       <c r="C144" s="1" t="n">
-        <v>59999</v>
+        <v>59974</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>426</v>
@@ -4172,7 +4253,7 @@
         <v>428</v>
       </c>
       <c r="C145" s="1" t="n">
-        <v>57543</v>
+        <v>59999</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>429</v>
@@ -4186,7 +4267,7 @@
         <v>431</v>
       </c>
       <c r="C146" s="1" t="n">
-        <v>60013</v>
+        <v>57543</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>432</v>
@@ -4200,7 +4281,7 @@
         <v>434</v>
       </c>
       <c r="C147" s="1" t="n">
-        <v>58201</v>
+        <v>60013</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>435</v>
@@ -4214,7 +4295,7 @@
         <v>437</v>
       </c>
       <c r="C148" s="1" t="n">
-        <v>59967</v>
+        <v>58201</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>438</v>
@@ -4228,7 +4309,7 @@
         <v>440</v>
       </c>
       <c r="C149" s="1" t="n">
-        <v>60056</v>
+        <v>59967</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>441</v>
@@ -4242,7 +4323,7 @@
         <v>443</v>
       </c>
       <c r="C150" s="1" t="n">
-        <v>59981</v>
+        <v>60056</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>444</v>
@@ -4256,10 +4337,24 @@
         <v>446</v>
       </c>
       <c r="C151" s="1" t="n">
-        <v>60009</v>
+        <v>59981</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>447</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C152" s="1" t="n">
+        <v>60009</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added fone EA43 Noah
</commit_message>
<xml_diff>
--- a/Proper Noun Dictionary (unicode1).xlsx
+++ b/Proper Noun Dictionary (unicode1).xlsx
@@ -1518,23 +1518,23 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{9BA6374C-279C-4354-8F60-35DD3333BD39}">
-  <header guid="{D4AA83B9-6A8F-4EF7-9077-C5C7714D311E}" dateTime="2018-08-22T16:48:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="55" maxSheetId="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{8B0D5097-C3A8-4AEB-9735-88E573CB7153}">
+  <header guid="{2A0F58B0-16C1-4E7D-B9F1-1399CB924933}" dateTime="2018-08-22T16:48:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="55" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{E8A03B13-6FD0-4AB8-8D12-18313A00E48C}" dateTime="2018-08-23T09:28:00.000000000Z" userName=" " r:id="rId2" minRId="56" maxRId="56" maxSheetId="2">
+  <header guid="{6179AAF9-A1F8-4978-868D-FCA4E99E42C9}" dateTime="2018-08-23T09:28:00.000000000Z" userName=" " r:id="rId2" minRId="56" maxRId="56" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{E9690B14-03D5-4742-9C0B-9FB635AB68A4}" dateTime="2018-08-23T16:56:00.000000000Z" userName=" " r:id="rId3" minRId="57" maxRId="59" maxSheetId="2">
+  <header guid="{B45643B4-32C3-4A98-AE9A-A183F5C692D0}" dateTime="2018-08-23T16:56:00.000000000Z" userName=" " r:id="rId3" minRId="57" maxRId="59" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{9BA6374C-279C-4354-8F60-35DD3333BD39}" dateTime="2018-08-23T16:57:00.000000000Z" userName=" " r:id="rId4" minRId="60" maxRId="61" maxSheetId="2">
+  <header guid="{8B0D5097-C3A8-4AEB-9735-88E573CB7153}" dateTime="2018-08-23T16:57:00.000000000Z" userName=" " r:id="rId4" minRId="60" maxRId="61" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -1544,16 +1544,16 @@
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rrc rId="1" ua="false" sId="1" eol="0" ref="170:170" action="insertRow"/>
-  <rrc rId="2" ua="false" sId="1" eol="0" ref="153:153" action="insertRow"/>
-  <rrc rId="3" ua="false" sId="1" eol="0" ref="147:147" action="insertRow"/>
-  <rrc rId="4" ua="false" sId="1" eol="0" ref="105:105" action="insertRow"/>
-  <rrc rId="5" ua="false" sId="1" eol="0" ref="88:88" action="insertRow"/>
-  <rrc rId="6" ua="false" sId="1" eol="0" ref="79:79" action="insertRow"/>
-  <rrc rId="7" ua="false" sId="1" eol="0" ref="68:68" action="insertRow"/>
-  <rrc rId="8" ua="false" sId="1" eol="0" ref="59:59" action="insertRow"/>
-  <rrc rId="9" ua="false" sId="1" eol="0" ref="35:35" action="insertRow"/>
-  <rrc rId="10" ua="false" sId="1" eol="0" ref="20:20" action="insertRow"/>
+  <rrc rId="1" ua="false" sId="1" eol="0" ref="181:181" action="insertRow"/>
+  <rrc rId="2" ua="false" sId="1" eol="0" ref="163:163" action="insertRow"/>
+  <rrc rId="3" ua="false" sId="1" eol="0" ref="156:156" action="insertRow"/>
+  <rrc rId="4" ua="false" sId="1" eol="0" ref="113:113" action="insertRow"/>
+  <rrc rId="5" ua="false" sId="1" eol="0" ref="94:94" action="insertRow"/>
+  <rrc rId="6" ua="false" sId="1" eol="0" ref="84:84" action="insertRow"/>
+  <rrc rId="7" ua="false" sId="1" eol="0" ref="72:72" action="insertRow"/>
+  <rrc rId="8" ua="false" sId="1" eol="0" ref="62:62" action="insertRow"/>
+  <rrc rId="9" ua="false" sId="1" eol="0" ref="37:37" action="insertRow"/>
+  <rrc rId="10" ua="false" sId="1" eol="0" ref="21:21" action="insertRow"/>
   <rrc rId="11" ua="false" sId="1" eol="0" ref="1:1" action="insertRow"/>
   <rcc rId="12" ua="false" sId="1">
     <nc r="A1" t="inlineStr">
@@ -1956,7 +1956,7 @@
     </nc>
   </rcc>
   <rcc rId="44" ua="false" sId="1">
-    <nc r="A131" t="inlineStr">
+    <nc r="A132" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -1971,7 +1971,7 @@
     </nc>
   </rcc>
   <rcc rId="45" ua="false" sId="1">
-    <nc r="B131" t="inlineStr">
+    <nc r="B132" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -1986,12 +1986,12 @@
     </nc>
   </rcc>
   <rcc rId="46" ua="false" sId="1">
-    <nc r="C131" t="n">
+    <nc r="C132" t="n">
       <v>60050</v>
     </nc>
   </rcc>
   <rcc rId="47" ua="false" sId="1">
-    <nc r="D131" t="inlineStr">
+    <nc r="D132" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2006,7 +2006,7 @@
     </nc>
   </rcc>
   <rcc rId="48" ua="false" sId="1">
-    <nc r="A135" t="inlineStr">
+    <nc r="A136" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2021,7 +2021,7 @@
     </nc>
   </rcc>
   <rcc rId="49" ua="false" sId="1">
-    <nc r="B135" t="inlineStr">
+    <nc r="B136" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2036,12 +2036,12 @@
     </nc>
   </rcc>
   <rcc rId="50" ua="false" sId="1">
-    <nc r="C135" t="n">
+    <nc r="C136" t="n">
       <v>60046</v>
     </nc>
   </rcc>
   <rcc rId="51" ua="false" sId="1">
-    <nc r="D135" t="inlineStr">
+    <nc r="D136" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2056,7 +2056,7 @@
     </nc>
   </rcc>
   <rcc rId="52" ua="false" sId="1">
-    <nc r="A150" t="inlineStr">
+    <nc r="A151" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2071,7 +2071,7 @@
     </nc>
   </rcc>
   <rcc rId="53" ua="false" sId="1">
-    <nc r="B150" t="inlineStr">
+    <nc r="B151" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2086,12 +2086,12 @@
     </nc>
   </rcc>
   <rcc rId="54" ua="false" sId="1">
-    <nc r="C150" t="n">
+    <nc r="C151" t="n">
       <v>60056</v>
     </nc>
   </rcc>
   <rcc rId="55" ua="false" sId="1">
-    <nc r="D150" t="inlineStr">
+    <nc r="D151" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2111,7 +2111,7 @@
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rcc rId="56" ua="false" sId="1">
-    <oc r="A131" t="inlineStr">
+    <oc r="A132" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2124,7 +2124,7 @@
         </r>
       </is>
     </oc>
-    <nc r="A131" t="inlineStr">
+    <nc r="A132" t="inlineStr">
       <is>
         <r>
           <rPr>
@@ -2150,9 +2150,8 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Noah</t>
@@ -2166,9 +2165,8 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve"></t>
@@ -2187,9 +2185,8 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
+            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">ea43</t>

</xml_diff>